<commit_message>
cull test code; other TODOs
</commit_message>
<xml_diff>
--- a/interface.xlsx
+++ b/interface.xlsx
@@ -13,17 +13,20 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1609900739" val="1024" rev="124" rev64="64" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1609900739" fixedDigits="0" showNotice="1" showProtection="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1609900739"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1609900739"/>
+      <pm:revision xmlns:pm="smNativeData" day="1609983593" val="1024" rev="124" rev64="64" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1609983593" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1609983593" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1609983593"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+  <si>
+    <t>Interface Type</t>
+  </si>
   <si>
     <t>SVG</t>
   </si>
@@ -40,7 +43,7 @@
     <t>Constructor Object</t>
   </si>
   <si>
-    <t>file type (language)</t>
+    <t>File type (language)</t>
   </si>
   <si>
     <t>*.view (SVG)</t>
@@ -103,22 +106,22 @@
     <t>.style.display</t>
   </si>
   <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>#position cx</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>#position cy</t>
+  </si>
+  <si>
     <t>Attribute</t>
   </si>
   <si>
-    <t>centerX</t>
-  </si>
-  <si>
-    <t>#position cx</t>
-  </si>
-  <si>
-    <t>centerY</t>
-  </si>
-  <si>
-    <t>#position cy</t>
-  </si>
-  <si>
-    <t>radius</t>
+    <t>r</t>
   </si>
   <si>
     <t>#position r</t>
@@ -130,25 +133,25 @@
     <t>If charAngle is set, assume mode=fix, otherwise mode=auto</t>
   </si>
   <si>
-    <t>textAnchor</t>
+    <t>text-anchor</t>
   </si>
   <si>
     <t>#text text-anchor</t>
   </si>
   <si>
-    <t>letterSpacing</t>
+    <t>letter-spacing</t>
   </si>
   <si>
     <t>#text letter-spacing</t>
   </si>
   <si>
-    <t>charAngle</t>
+    <t>sweep-angle (charAngle)</t>
   </si>
   <si>
     <t>#orientation sweep-angle</t>
   </si>
   <si>
-    <t>rotateText</t>
+    <t>start-angle (rotateText)</t>
   </si>
   <si>
     <t>#orientation start-angle</t>
@@ -157,7 +160,7 @@
     <t>.startAngle OR .anchorAngle</t>
   </si>
   <si>
-    <t>className</t>
+    <t>class</t>
   </si>
   <si>
     <t>#text class</t>
@@ -185,7 +188,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1609900739" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1609983593" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -201,7 +204,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1609900739" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1609983593" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -210,7 +213,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,11 +222,88 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1609983593" type="1" fgLvl="100" fgClr="0000FF00" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1609983593" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1609983593" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609900739" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1609983593" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF9E"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1609983593" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808001"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1609983593" type="1" fgLvl="50" fgClr="00FFFF00" bgLvl="50" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA3A300"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1609983593" type="1" fgLvl="64" fgClr="00FFFF00" bgLvl="36" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD1D100"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1609983593" type="1" fgLvl="82" fgClr="00FFFF00" bgLvl="18" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -234,18 +314,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609900739" type="1" fgLvl="50" fgClr="0000FF00" bgLvl="50" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00A300"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609900739" type="1" fgLvl="64" fgClr="0000FF00" bgLvl="36" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1609983593" type="1" fgLvl="50" fgClr="0000FF00" bgLvl="50" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -256,101 +325,13 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609900739" type="1" fgLvl="82" fgClr="0000FF00" bgLvl="18" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00FF00"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609900739" type="1" fgLvl="100" fgClr="0000FF00" bgLvl="0" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF800101"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609900739" type="1" fgLvl="50" fgClr="00FF0000" bgLvl="50" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA30000"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609900739" type="1" fgLvl="64" fgClr="00FF0000" bgLvl="36" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA3A300"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609900739" type="1" fgLvl="64" fgClr="00FFFF00" bgLvl="36" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD1D100"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609900739" type="1" fgLvl="82" fgClr="00FFFF00" bgLvl="18" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD10000"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609900739" type="1" fgLvl="82" fgClr="00FF0000" bgLvl="18" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609900739" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609900739" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1609983593" type="1" fgLvl="82" fgClr="0000FF00" bgLvl="18" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -366,7 +347,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609900739"/>
+          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
         </ext>
       </extLst>
     </border>
@@ -385,7 +366,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609900739"/>
+          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
         </ext>
       </extLst>
     </border>
@@ -404,7 +385,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609900739"/>
+          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
         </ext>
       </extLst>
     </border>
@@ -423,7 +404,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609900739"/>
+          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
         </ext>
       </extLst>
     </border>
@@ -442,7 +423,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609900739"/>
+          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
         </ext>
       </extLst>
     </border>
@@ -461,7 +442,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609900739"/>
+          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
         </ext>
       </extLst>
     </border>
@@ -480,7 +461,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609900739"/>
+          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
         </ext>
       </extLst>
     </border>
@@ -499,7 +480,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609900739"/>
+          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
         </ext>
       </extLst>
     </border>
@@ -518,7 +499,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609900739"/>
+          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
         </ext>
       </extLst>
     </border>
@@ -537,7 +518,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609900739"/>
+          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
         </ext>
       </extLst>
     </border>
@@ -556,45 +537,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609900739"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609900739"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609900739"/>
+          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
         </ext>
       </extLst>
     </border>
@@ -602,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -623,22 +566,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -648,9 +585,19 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1609900739" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1609983593" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
+      <pm:colors xmlns:pm="smNativeData" id="1609983593" count="8">
+        <pm:color name="Colour 24" rgb="018001"/>
+        <pm:color name="Colour 25" rgb="00A300"/>
+        <pm:color name="Colour 26" rgb="00D100"/>
+        <pm:color name="Colour 27" rgb="800101"/>
+        <pm:color name="Colour 28" rgb="A30000"/>
+        <pm:color name="Colour 29" rgb="A3A300"/>
+        <pm:color name="Colour 30" rgb="D1D100"/>
+        <pm:color name="Colour 31" rgb="D10000"/>
+      </pm:colors>
     </ext>
   </extLst>
 </styleSheet>
@@ -915,240 +862,242 @@
   <dimension ref="A3:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
   <cols>
     <col min="1" max="1" width="9.864865" customWidth="1" style="4"/>
-    <col min="2" max="2" width="17.432432" customWidth="1" style="4"/>
-    <col min="3" max="7" width="16.486486" customWidth="1" style="9"/>
+    <col min="2" max="2" width="17.432432" customWidth="1" style="7"/>
+    <col min="3" max="7" width="16.486486" customWidth="1" style="7"/>
     <col min="8" max="16384" width="16.486486" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:7" s="1" customFormat="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="11" t="s">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="D3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="E3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="F3" s="6" t="s">
         <v>4</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="3" customFormat="1">
       <c r="A4" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1">
       <c r="A5" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="12"/>
+      <c r="F6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="12"/>
+      <c r="B7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="12"/>
+      <c r="B8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="B9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="12"/>
+      <c r="C9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="B10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="12"/>
+      <c r="C10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="10" t="s">
+      <c r="B11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="12"/>
+      <c r="C11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="12"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" spans="2:7">
-      <c r="B14" s="4" t="s">
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="B14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="1:7" s="8" customFormat="1">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" s="2" customFormat="1">
+      <c r="A15" s="7"/>
+      <c r="B15" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="12"/>
+      <c r="C15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="10"/>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="10" t="s">
+      <c r="B16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="12"/>
+      <c r="C16" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="10" t="s">
+      <c r="B17" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="12"/>
+      <c r="C17" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="10" t="s">
+      <c r="B18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="12"/>
+      <c r="C18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="10" t="s">
+      <c r="B19" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="C19" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="12"/>
+      <c r="F19" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="9"/>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="10" t="s">
+      <c r="B20" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G20" s="12"/>
+      <c r="C20" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="9"/>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1609900739" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1609983593" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1157,16 +1106,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1609900739" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1609900739" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1609900739" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1609900739" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1609983593" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1609983593" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1609983593" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1609983593" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1609900739" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1609983593" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
get SVG attributes working and documented
</commit_message>
<xml_diff>
--- a/interface.xlsx
+++ b/interface.xlsx
@@ -13,17 +13,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1609983593" val="1024" rev="124" rev64="64" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1609983593" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1609983593" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1609983593"/>
+      <pm:revision xmlns:pm="smNativeData" day="1610079960" val="1024" rev="124" rev64="64" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1610079960" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1610079960" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1610079960"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>Interface Type</t>
   </si>
@@ -91,6 +91,9 @@
     <t>fill</t>
   </si>
   <si>
+    <t>.fill</t>
+  </si>
+  <si>
     <t>.style.fill</t>
   </si>
   <si>
@@ -164,6 +167,9 @@
   </si>
   <si>
     <t>#text class</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -188,7 +194,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1609983593" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1610079960" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -204,7 +210,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1609983593" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1610079960" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -213,7 +219,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,7 +232,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609983593" type="1" fgLvl="100" fgClr="0000FF00" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610079960" type="1" fgLvl="100" fgClr="0000FF00" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -237,7 +243,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609983593" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610079960" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -248,7 +254,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609983593" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610079960" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -259,18 +265,73 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609983593" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF9E"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609983593" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610079960" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF800101"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610079960" type="1" fgLvl="50" fgClr="00FF0000" bgLvl="50" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA30000"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610079960" type="1" fgLvl="64" fgClr="00FF0000" bgLvl="36" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD10000"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610079960" type="1" fgLvl="82" fgClr="00FF0000" bgLvl="18" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3D3D"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610079960" type="1" fgLvl="76" fgClr="00FF0000" bgLvl="24" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5C5C"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610079960" type="1" fgLvl="64" fgClr="00FF0000" bgLvl="36" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9E9E"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610079960" type="1" fgLvl="38" fgClr="00FF0000" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -281,7 +342,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609983593" type="1" fgLvl="50" fgClr="00FFFF00" bgLvl="50" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610079960" type="1" fgLvl="50" fgClr="00FFFF00" bgLvl="50" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -292,252 +353,437 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609983593" type="1" fgLvl="64" fgClr="00FFFF00" bgLvl="36" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD1D100"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609983593" type="1" fgLvl="82" fgClr="00FFFF00" bgLvl="18" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF018001"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609983593" type="1" fgLvl="50" fgClr="0000FF00" bgLvl="50" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00D100"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1609983593" type="1" fgLvl="82" fgClr="0000FF00" bgLvl="18" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610079960" type="1" fgLvl="64" fgClr="00FFFF00" bgLvl="36" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3DFF3D"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610079960" type="1" fgLvl="76" fgClr="0000FF00" bgLvl="24" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5CFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610079960" type="1" fgLvl="64" fgClr="0000FFFF" bgLvl="36" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9E9EFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610079960" type="1" fgLvl="38" fgClr="000000FF" bgLvl="62" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE0FF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610079960" type="1" fgLvl="12" fgClr="00FF00FF" bgLvl="88" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0F0E0"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610079960" type="1" fgLvl="12" fgClr="007F7F00" bgLvl="88" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610079960" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1609983593"/>
+  <borders count="19">
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610079960"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610079960"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610079960"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610079960"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610079960"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610079960"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610079960"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610079960"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610079960"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610079960"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610079960"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610079960"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610079960"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610079960"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610079960"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610079960"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610079960"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610079960"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610079960"/>
         </ext>
       </extLst>
     </border>
@@ -545,7 +791,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -575,7 +821,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="18" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -585,10 +834,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1609983593" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1610079960" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1609983593" count="8">
+      <pm:colors xmlns:pm="smNativeData" id="1610079960" count="10">
         <pm:color name="Colour 24" rgb="018001"/>
         <pm:color name="Colour 25" rgb="00A300"/>
         <pm:color name="Colour 26" rgb="00D100"/>
@@ -597,6 +846,8 @@
         <pm:color name="Colour 29" rgb="A3A300"/>
         <pm:color name="Colour 30" rgb="D1D100"/>
         <pm:color name="Colour 31" rgb="D10000"/>
+        <pm:color name="Colour 32" rgb="FFFF9E"/>
+        <pm:color name="Colour 33" rgb="808001"/>
       </pm:colors>
     </ext>
   </extLst>
@@ -862,7 +1113,7 @@
   <dimension ref="A3:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -971,125 +1222,131 @@
         <v>21</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="2:7">
       <c r="B12" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="8" t="s">
         <v>28</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="G12" s="9"/>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="8" t="s">
         <v>30</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7" s="2" customFormat="1">
       <c r="A15" s="7"/>
-      <c r="B15" s="11" t="s">
-        <v>34</v>
+      <c r="B15" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
+        <v>36</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
       <c r="G15" s="10"/>
     </row>
     <row r="16" spans="2:7">
       <c r="B16" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G16" s="9"/>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G17" s="9"/>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G18" s="9"/>
     </row>
     <row r="19" spans="2:7">
       <c r="B19" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G19" s="9"/>
     </row>
     <row r="20" spans="2:7">
       <c r="B20" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="G20" s="9"/>
     </row>
@@ -1097,7 +1354,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1609983593" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1610079960" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1106,16 +1363,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1609983593" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1609983593" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1609983593" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1609983593" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1610079960" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1610079960" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1610079960" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1610079960" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1609983593" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1610079960" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
forgot to save the xlsx
</commit_message>
<xml_diff>
--- a/interface.xlsx
+++ b/interface.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="53">
   <si>
     <t xml:space="preserve">Interface Type</t>
   </si>
@@ -34,7 +34,10 @@
     <t xml:space="preserve">CSS by class</t>
   </si>
   <si>
-    <t xml:space="preserve">API</t>
+    <t xml:space="preserve">API by id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API by class</t>
   </si>
   <si>
     <t xml:space="preserve">Constructor Object</t>
@@ -85,6 +88,9 @@
     <t xml:space="preserve">font-family</t>
   </si>
   <si>
+    <t xml:space="preserve">.style.fontFamily</t>
+  </si>
+  <si>
     <t xml:space="preserve">font-size</t>
   </si>
   <si>
@@ -169,8 +175,11 @@
     <t xml:space="preserve">#text class</t>
   </si>
   <si>
-    <t xml:space="preserve">* looks as if we don´t reach #position/#orientation from CSS (maybe still, as they´re outside the SVG in the symbol?
-I had changed it to a &lt;g&gt; with no luck re reaching it. Changed back)</t>
+    <t xml:space="preserve">* looks as if we don´t reach #position/#orientation from CSS 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">** if settings on different levels: SVG &gt; CSS &gt; .ts/.js</t>
   </si>
 </sst>
 </file>
@@ -180,7 +189,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -210,12 +219,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -284,7 +287,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -321,7 +324,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -337,8 +340,12 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -418,20 +425,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:G1048576"/>
+  <dimension ref="A3:H24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5078125" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="3" style="2" width="16.48"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="3" style="2" width="16.48"/>
   </cols>
   <sheetData>
-    <row r="3" s="4" customFormat="true" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -451,293 +458,321 @@
       <c r="G3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" s="5" customFormat="true" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" s="6" customFormat="true" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" s="6" customFormat="true" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H5" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="8"/>
+        <v>21</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="H8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="8"/>
+        <v>26</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="8"/>
+        <v>28</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="8"/>
+        <v>30</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="8"/>
+        <v>19</v>
+      </c>
+      <c r="H12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="8"/>
+        <v>19</v>
+      </c>
+      <c r="H13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="8"/>
+        <v>19</v>
+      </c>
+      <c r="H14" s="8"/>
     </row>
     <row r="15" s="6" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
       <c r="B15" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="8"/>
+        <v>19</v>
+      </c>
+      <c r="H16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="8"/>
+        <v>19</v>
+      </c>
+      <c r="H17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="8"/>
+        <v>19</v>
+      </c>
+      <c r="H18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>48</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="8"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="8"/>
+        <v>19</v>
+      </c>
+      <c r="H20" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -745,12 +780,24 @@
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="H23" s="13"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A23:G23"/>
+  <mergeCells count="2">
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="A24:H24"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
use x,y not cx,cy; test; document
</commit_message>
<xml_diff>
--- a/interface.xlsx
+++ b/interface.xlsx
@@ -13,17 +13,17 @@
   <calcPr iterateDelta="0.0001"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1610154436" val="1024" rev="124" rev64="64" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1610154436" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1610154436" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1610154436"/>
+      <pm:revision xmlns:pm="smNativeData" day="1610156659" val="1024" rev="124" rev64="64" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1610156659" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1610156659" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1610156659"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="56">
   <si>
     <t>Interface Type</t>
   </si>
@@ -88,12 +88,12 @@
     <t>.text</t>
   </si>
   <si>
+    <t>Not implemented</t>
+  </si>
+  <si>
     <t>font-family</t>
   </si>
   <si>
-    <t>Not implemented</t>
-  </si>
-  <si>
     <t>font-size</t>
   </si>
   <si>
@@ -121,13 +121,13 @@
     <t>x</t>
   </si>
   <si>
-    <t>#position cx</t>
+    <t>.x</t>
   </si>
   <si>
     <t>y</t>
   </si>
   <si>
-    <t>#position cy</t>
+    <t>.y</t>
   </si>
   <si>
     <t>Attribute</t>
@@ -221,7 +221,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1610154436" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1610156659" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -237,7 +237,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1610154436" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1610156659" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="200" lang="default" weight="bold"/>
@@ -246,7 +246,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="46">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,7 +259,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610154436" type="1" fgLvl="100" fgClr="0000FF00" bgLvl="0" bgClr="0033CCCC"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="0000FF00" bgLvl="0" bgClr="0033CCCC"/>
           </ext>
         </extLst>
       </patternFill>
@@ -270,7 +270,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610154436" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00FF3D3D"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00FF3D3D"/>
           </ext>
         </extLst>
       </patternFill>
@@ -281,7 +281,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610154436" type="1" fgLvl="100" fgClr="00FF3D3D" bgLvl="0" bgClr="00FF0000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="00FF3D3D" bgLvl="0" bgClr="00FF0000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -292,7 +292,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610154436" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00FFFF00"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00FFFF00"/>
           </ext>
         </extLst>
       </patternFill>
@@ -303,7 +303,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610154436" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -314,7 +314,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610154436" type="1" fgLvl="50" fgClr="0000FF00" bgLvl="50" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="50" fgClr="0000FF00" bgLvl="50" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -325,7 +325,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610154436" type="1" fgLvl="82" fgClr="0000FF00" bgLvl="18" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="82" fgClr="0000FF00" bgLvl="18" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -336,7 +336,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610154436" type="1" fgLvl="76" fgClr="0000FF00" bgLvl="24" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="76" fgClr="0000FF00" bgLvl="24" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -347,7 +347,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610154436" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -358,7 +358,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610154436" type="1" fgLvl="100" fgClr="000000FF" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="000000FF" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -369,7 +369,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610154436" type="1" fgLvl="100" fgClr="00007F7F" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="00007F7F" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -380,257 +380,1217 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610154436" type="1" fgLvl="100" fgClr="00E6E6E6" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="00E6E6E6" bgLvl="0" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00A3A3"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="64" fgClr="0000FFFF" bgLvl="36" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00D1D1"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="82" fgClr="0000FFFF" bgLvl="18" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="0000FF00" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="0000FFFF" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3D3DFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="76" fgClr="000000FF" bgLvl="24" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5C5CFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="64" fgClr="000000FF" bgLvl="36" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9E9EFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="38" fgClr="000000FF" bgLvl="62" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE0E0FF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="12" fgClr="000000FF" bgLvl="88" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="00FF00FF" bgLvl="0" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE0FFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="12" fgClr="0000FFFF" bgLvl="88" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE0FFE0"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="12" fgClr="0000FF00" bgLvl="88" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9EFF9E"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="38" fgClr="0000FF00" bgLvl="62" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5CFF5C"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="64" fgClr="0000FF00" bgLvl="36" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF3D"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="76" fgClr="00FFFF00" bgLvl="24" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD10000"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="82" fgClr="00FF0000" bgLvl="18" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA30000"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="64" fgClr="00FF0000" bgLvl="36" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF800101"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="50" fgClr="00FF0000" bgLvl="50" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF5C"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="64" fgClr="00FFFF00" bgLvl="36" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFE0"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="12" fgClr="00FFFF00" bgLvl="88" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="0000FF00" bgLvl="0" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808001"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="50" fgClr="00FFFF00" bgLvl="50" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA3A300"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="64" fgClr="00FFFF00" bgLvl="36" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD1D100"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="82" fgClr="00FFFF00" bgLvl="18" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9EFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="38" fgClr="0000FFFF" bgLvl="62" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF010180"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="50" fgClr="000000FF" bgLvl="50" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000A3"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="64" fgClr="000000FF" bgLvl="36" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000D1"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="82" fgClr="000000FF" bgLvl="18" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="000000FF" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5CFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="64" fgClr="0000FFFF" bgLvl="36" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610154436"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610154436"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610154436"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610154436"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610154436"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610154436"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610154436"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610154436"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610154436"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610154436"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610154436"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610154436"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610154436"/>
+  <borders count="45">
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
         </ext>
       </extLst>
     </border>
@@ -643,7 +1603,7 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2"/>
@@ -669,12 +1629,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -693,6 +1647,24 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="21" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="28" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="21" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -705,10 +1677,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1610154436" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1610156659" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1610154436" count="2">
+      <pm:colors xmlns:pm="smNativeData" id="1610156659" count="2">
         <pm:color name="Colour 24" rgb="33CCCC"/>
         <pm:color name="Colour 25" rgb="FF3D3D"/>
       </pm:colors>
@@ -976,7 +1948,7 @@
   <dimension ref="A3:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="15" defaultColWidth="16.531532" defaultRowHeight="13.45"/>
@@ -1065,10 +2037,10 @@
       <c r="C6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="24" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="12" t="s">
@@ -1077,28 +2049,32 @@
       <c r="G6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="13"/>
+      <c r="H6" s="21" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="D7" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="13"/>
+      <c r="E7" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="2:8">
       <c r="B8" s="7" t="s">
@@ -1107,19 +2083,21 @@
       <c r="C8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="13"/>
+      <c r="F8" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="2:8">
       <c r="B9" s="7" t="s">
@@ -1128,10 +2106,10 @@
       <c r="C9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="20" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="12" t="s">
@@ -1140,7 +2118,9 @@
       <c r="G9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="13"/>
+      <c r="H9" s="21" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="2:8">
       <c r="B10" s="7" t="s">
@@ -1149,10 +2129,10 @@
       <c r="C10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="20" t="s">
         <v>27</v>
       </c>
       <c r="F10" s="12" t="s">
@@ -1161,7 +2141,9 @@
       <c r="G10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="13"/>
+      <c r="H10" s="21" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="7" t="s">
@@ -1170,10 +2152,10 @@
       <c r="C11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="20" t="s">
         <v>29</v>
       </c>
       <c r="F11" s="12" t="s">
@@ -1182,52 +2164,58 @@
       <c r="G11" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="13"/>
+      <c r="H11" s="21" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="2:8">
       <c r="B12" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="13"/>
+      <c r="G12" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="2:8">
       <c r="B13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="13"/>
+      <c r="G13" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -1236,33 +2224,37 @@
       <c r="C14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="13"/>
+      <c r="F14" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:8" s="11" customFormat="1">
       <c r="A15" s="7"/>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="21" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="7" t="s">
@@ -1271,19 +2263,21 @@
       <c r="C16" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="13"/>
+      <c r="F16" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="17" spans="2:8">
       <c r="B17" s="7" t="s">
@@ -1292,19 +2286,21 @@
       <c r="C17" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" s="13"/>
+      <c r="F17" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="18" spans="2:8">
       <c r="B18" s="7" t="s">
@@ -1313,19 +2309,21 @@
       <c r="C18" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="13"/>
+      <c r="F18" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="19" spans="2:8">
       <c r="B19" s="7" t="s">
@@ -1334,10 +2332,10 @@
       <c r="C19" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="17" t="s">
         <v>19</v>
       </c>
       <c r="F19" s="12" t="s">
@@ -1346,7 +2344,9 @@
       <c r="G19" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="13"/>
+      <c r="H19" s="21" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="20" spans="2:8">
       <c r="B20" s="7" t="s">
@@ -1355,51 +2355,53 @@
       <c r="C20" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="H20" s="13"/>
+      <c r="H20" s="21" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="23" spans="1:8" ht="23.85" customHeight="1">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="16" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="18" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1411,7 +2413,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1610154436" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1610156659" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1420,16 +2422,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1610154436" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1610154436" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1610154436" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1610154436" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1610156659" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1610156659" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1610156659" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1610156659" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1610154436" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1610156659" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
r via CSS class
</commit_message>
<xml_diff>
--- a/interface.xlsx
+++ b/interface.xlsx
@@ -13,17 +13,17 @@
   <calcPr iterateDelta="0.0001"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1610156659" val="1024" rev="124" rev64="64" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1610156659" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1610156659" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1610156659"/>
+      <pm:revision xmlns:pm="smNativeData" day="1610158738" val="1024" rev="124" rev64="64" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1610158738" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1610158738" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1610158738"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="58">
   <si>
     <t>Interface Type</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>#position r</t>
+  </si>
+  <si>
+    <t>#id #position</t>
+  </si>
+  <si>
+    <t>.className #position</t>
   </si>
   <si>
     <t>mode</t>
@@ -221,7 +227,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1610156659" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1610158738" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -237,7 +243,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1610156659" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1610158738" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="200" lang="default" weight="bold"/>
@@ -246,7 +252,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="46">
+  <fills count="48">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,7 +265,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="0000FF00" bgLvl="0" bgClr="0033CCCC"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="100" fgClr="0000FF00" bgLvl="0" bgClr="0033CCCC"/>
           </ext>
         </extLst>
       </patternFill>
@@ -270,7 +276,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00FF3D3D"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00FF3D3D"/>
           </ext>
         </extLst>
       </patternFill>
@@ -281,7 +287,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="00FF3D3D" bgLvl="0" bgClr="00FF0000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="100" fgClr="00FF3D3D" bgLvl="0" bgClr="00FF0000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -292,7 +298,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00FFFF00"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00FFFF00"/>
           </ext>
         </extLst>
       </patternFill>
@@ -303,7 +309,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -314,7 +320,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="50" fgClr="0000FF00" bgLvl="50" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="50" fgClr="0000FF00" bgLvl="50" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -325,7 +331,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="82" fgClr="0000FF00" bgLvl="18" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="82" fgClr="0000FF00" bgLvl="18" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -336,7 +342,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="76" fgClr="0000FF00" bgLvl="24" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="76" fgClr="0000FF00" bgLvl="24" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -347,7 +353,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -358,7 +364,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="000000FF" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="100" fgClr="000000FF" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -369,7 +375,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="00007F7F" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="100" fgClr="00007F7F" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -380,7 +386,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="00E6E6E6" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="100" fgClr="00E6E6E6" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -391,7 +397,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="64" fgClr="0000FFFF" bgLvl="36" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="64" fgClr="0000FFFF" bgLvl="36" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -402,7 +408,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="82" fgClr="0000FFFF" bgLvl="18" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="82" fgClr="0000FFFF" bgLvl="18" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -413,7 +419,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="0000FF00" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="100" fgClr="0000FF00" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -424,7 +430,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="0000FFFF" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="100" fgClr="0000FFFF" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -435,7 +441,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="76" fgClr="000000FF" bgLvl="24" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="76" fgClr="000000FF" bgLvl="24" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -446,7 +452,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="64" fgClr="000000FF" bgLvl="36" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="64" fgClr="000000FF" bgLvl="36" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -457,7 +463,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="38" fgClr="000000FF" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="38" fgClr="000000FF" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -468,7 +474,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="12" fgClr="000000FF" bgLvl="88" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="12" fgClr="000000FF" bgLvl="88" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -479,7 +485,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -490,7 +496,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="00FF00FF" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="100" fgClr="00FF00FF" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -501,7 +507,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="12" fgClr="0000FFFF" bgLvl="88" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="12" fgClr="0000FFFF" bgLvl="88" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -512,7 +518,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="12" fgClr="0000FF00" bgLvl="88" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="12" fgClr="0000FF00" bgLvl="88" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -523,7 +529,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="38" fgClr="0000FF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="38" fgClr="0000FF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -534,7 +540,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="64" fgClr="0000FF00" bgLvl="36" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="64" fgClr="0000FF00" bgLvl="36" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -545,7 +551,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="76" fgClr="00FFFF00" bgLvl="24" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="76" fgClr="00FFFF00" bgLvl="24" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -556,7 +562,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -567,7 +573,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="82" fgClr="00FF0000" bgLvl="18" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="82" fgClr="00FF0000" bgLvl="18" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -578,7 +584,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="64" fgClr="00FF0000" bgLvl="36" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="64" fgClr="00FF0000" bgLvl="36" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -589,7 +595,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="50" fgClr="00FF0000" bgLvl="50" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="50" fgClr="00FF0000" bgLvl="50" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -600,7 +606,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -611,7 +617,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="64" fgClr="00FFFF00" bgLvl="36" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="64" fgClr="00FFFF00" bgLvl="36" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -622,7 +628,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="12" fgClr="00FFFF00" bgLvl="88" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="12" fgClr="00FFFF00" bgLvl="88" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -633,7 +639,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="0000FF00" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="100" fgClr="0000FF00" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -644,7 +650,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="50" fgClr="00FFFF00" bgLvl="50" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="50" fgClr="00FFFF00" bgLvl="50" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -655,7 +661,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="64" fgClr="00FFFF00" bgLvl="36" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="64" fgClr="00FFFF00" bgLvl="36" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -666,7 +672,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="82" fgClr="00FFFF00" bgLvl="18" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="82" fgClr="00FFFF00" bgLvl="18" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -677,7 +683,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="38" fgClr="0000FFFF" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="38" fgClr="0000FFFF" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -688,7 +694,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="50" fgClr="000000FF" bgLvl="50" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="50" fgClr="000000FF" bgLvl="50" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -699,7 +705,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="64" fgClr="000000FF" bgLvl="36" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="64" fgClr="000000FF" bgLvl="36" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -710,7 +716,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="82" fgClr="000000FF" bgLvl="18" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="82" fgClr="000000FF" bgLvl="18" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -721,7 +727,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="100" fgClr="000000FF" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="100" fgClr="000000FF" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -732,865 +738,925 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1610156659" type="1" fgLvl="64" fgClr="0000FFFF" bgLvl="36" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="64" fgClr="0000FFFF" bgLvl="36" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00A300"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="64" fgClr="0000FF00" bgLvl="36" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3DFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1610158738" type="1" fgLvl="76" fgClr="0000FFFF" bgLvl="24" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1610156659"/>
+  <borders count="47">
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1610158738"/>
         </ext>
       </extLst>
     </border>
@@ -1603,7 +1669,7 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2"/>
@@ -1665,6 +1731,9 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="35" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -1677,10 +1746,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1610156659" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1610158738" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1610156659" count="2">
+      <pm:colors xmlns:pm="smNativeData" id="1610158738" count="2">
         <pm:color name="Colour 24" rgb="33CCCC"/>
         <pm:color name="Colour 25" rgb="FF3D3D"/>
       </pm:colors>
@@ -1948,7 +2017,7 @@
   <dimension ref="A3:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="15" defaultColWidth="16.531532" defaultRowHeight="13.45"/>
@@ -2224,11 +2293,11 @@
       <c r="C14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>19</v>
+      <c r="D14" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>39</v>
       </c>
       <c r="F14" s="21" t="s">
         <v>21</v>
@@ -2243,10 +2312,10 @@
     <row r="15" spans="1:8" s="11" customFormat="1">
       <c r="A15" s="7"/>
       <c r="B15" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
@@ -2258,10 +2327,10 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>19</v>
@@ -2281,10 +2350,10 @@
     </row>
     <row r="17" spans="2:8">
       <c r="B17" s="7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>19</v>
@@ -2304,10 +2373,10 @@
     </row>
     <row r="18" spans="2:8">
       <c r="B18" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>19</v>
@@ -2327,10 +2396,10 @@
     </row>
     <row r="19" spans="2:8">
       <c r="B19" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>19</v>
@@ -2339,10 +2408,10 @@
         <v>19</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H19" s="21" t="s">
         <v>21</v>
@@ -2350,10 +2419,10 @@
     </row>
     <row r="20" spans="2:8">
       <c r="B20" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D20" s="23" t="s">
         <v>19</v>
@@ -2362,10 +2431,10 @@
         <v>19</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H20" s="21" t="s">
         <v>21</v>
@@ -2373,7 +2442,7 @@
     </row>
     <row r="23" spans="1:8" ht="23.85" customHeight="1">
       <c r="A23" s="15" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -2385,7 +2454,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="16" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
@@ -2397,12 +2466,12 @@
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="16" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2413,7 +2482,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1610156659" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1610158738" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2422,16 +2491,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1610156659" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1610156659" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1610156659" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1610156659" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1610158738" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1610158738" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1610158738" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1610158738" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1610156659" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1610158738" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
rearranged xlsx (to update after renaming vars)
</commit_message>
<xml_diff>
--- a/interface.xlsx
+++ b/interface.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="63">
   <si>
     <t xml:space="preserve">Interface Type</t>
   </si>
@@ -55,21 +55,75 @@
     <t xml:space="preserve">Usage</t>
   </si>
   <si>
-    <t xml:space="preserve">Apply inline; ie, within &lt;use&gt;, possibly requiring &lt;set&gt;.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apply to widgets by id via #id {...}.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apply to widgets by class via .class {...}. May require widgets to acquire class indirectly; eg,  &lt;set href="#text" attributeName="class" to="myClass" /&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call a property setter or function.</t>
+    <t xml:space="preserve">Apply in &lt;use&gt;*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apply by id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apply by class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call </t>
   </si>
   <si>
     <t xml:space="preserve">Object attribute:value pair passed to constructor. Non-standard; not implemented.</t>
   </si>
   <si>
+    <t xml:space="preserve">font-family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.style.fontFamily</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not implemented</t>
+  </si>
+  <si>
+    <t xml:space="preserve">font-size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.style.fontSize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.fill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.style.fill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.style.opacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.style.display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apply via &lt;set&gt;**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specified selector</t>
+  </si>
+  <si>
     <t xml:space="preserve">text</t>
   </si>
   <si>
@@ -85,61 +139,13 @@
     <t xml:space="preserve">.text</t>
   </si>
   <si>
-    <t xml:space="preserve">Not implemented</t>
-  </si>
-  <si>
-    <t xml:space="preserve">font-family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.style.fontFamily</t>
-  </si>
-  <si>
-    <t xml:space="preserve">font-size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.style.fontSize</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.fill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.style.fill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">opacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.style.opacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.style.display</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.y</t>
-  </si>
-  <si>
     <t xml:space="preserve">Attribute</t>
   </si>
   <si>
     <t xml:space="preserve">r</t>
   </si>
   <si>
-    <t xml:space="preserve">#position r</t>
+    <t xml:space="preserve">#radius r</t>
   </si>
   <si>
     <t xml:space="preserve">#id #radius</t>
@@ -169,7 +175,7 @@
     <t xml:space="preserve">sweep-angle (charAngle)</t>
   </si>
   <si>
-    <t xml:space="preserve">#orientation sweep-angle</t>
+    <t xml:space="preserve">#layout sweep-angle</t>
   </si>
   <si>
     <t xml:space="preserve">#id #layout</t>
@@ -181,7 +187,7 @@
     <t xml:space="preserve">start-angle (rotateText)</t>
   </si>
   <si>
-    <t xml:space="preserve">#orientation start-angle</t>
+    <t xml:space="preserve">#layout  start-angle</t>
   </si>
   <si>
     <t xml:space="preserve">.startAngle OR .anchorAngle</t>
@@ -304,7 +310,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -343,6 +349,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -370,17 +380,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:G26"/>
+  <dimension ref="A3:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.58984375" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.61328125" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="2" width="16.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="2" width="16.48"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="7" min="7" style="2" width="16.48"/>
   </cols>
   <sheetData>
     <row r="3" s="4" customFormat="true" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -425,243 +436,238 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" s="6" customFormat="true" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="6" customFormat="true" ht="13.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>20</v>
-      </c>
       <c r="G6" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="7" t="s">
+      <c r="D8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>25</v>
-      </c>
       <c r="G8" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="E13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="7" t="s">
+      <c r="F13" s="10"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="2" t="s">
+      <c r="C14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
+      <c r="E14" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="F14" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="G14" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="B15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="C15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" s="6" customFormat="true" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2"/>
-      <c r="B15" s="10" t="s">
+      <c r="D15" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="E15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
+      <c r="F15" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="G15" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" s="6" customFormat="true" ht="13.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2"/>
+      <c r="B16" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
       <c r="G16" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -672,16 +678,16 @@
         <v>47</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,75 +698,96 @@
         <v>49</v>
       </c>
       <c r="D18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="C19" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="2" t="s">
+      <c r="D19" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G19" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="G20" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="F20" s="10" t="s">
+      <c r="C21" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="G20" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11" t="s">
+      <c r="D21" s="8" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11" t="s">
+      <c r="E21" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" s="11" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11"/>
-    </row>
+      <c r="G21" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="12"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="portrait" blackAndWhite="false" draft="false" cellComments="atEnd" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>